<commit_message>
Add XLSX to HTML converter with complete reproducibility
- Create all-in-one Python script for converting XLSX data to HTML JavaScript arrays
- Add comprehensive error handling and automatic newline character fixing
- Include configuration file support and detailed documentation
- Update HTML file with properly escaped data from Excel source
- Ensure complete reproducibility across multiple executions

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/woman-excel.xlsx
+++ b/woman-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wankuma-my.sharepoint.com/personal/naka_wankuma_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="6_{B69F568A-D26F-4418-9710-6ADC08CBB386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED5306EA-3D19-4CFF-A38A-2B76B1C3BDE0}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="6_{B69F568A-D26F-4418-9710-6ADC08CBB386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D98426-F947-41E5-899B-BFDA0F4288FA}"/>
   <bookViews>
-    <workbookView xWindow="-67" yWindow="-67" windowWidth="25734" windowHeight="13814" xr2:uid="{006E6351-9C88-4E01-B808-191D08DA05AD}"/>
+    <workbookView xWindow="25533" yWindow="-67" windowWidth="25734" windowHeight="13814" xr2:uid="{006E6351-9C88-4E01-B808-191D08DA05AD}"/>
   </bookViews>
   <sheets>
     <sheet name="現役選手デビュー年団体別一覧" sheetId="1" r:id="rId1"/>
@@ -1210,20 +1210,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ハミングバード
-メガトン
-後藤智香
-天麗皇希
-山田奈保</t>
-    <rPh sb="13" eb="17">
-      <t>ゴトウチカ</t>
-    </rPh>
-    <rPh sb="18" eb="22">
-      <t>アマレイコウキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>伊藤麻希
 小橋マリカ</t>
     <phoneticPr fontId="1"/>
@@ -1298,14 +1284,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>梨央
-(弥福かな)</t>
-    <rPh sb="0" eb="2">
-      <t>リオ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>JENNE</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1321,17 +1299,6 @@
   </si>
   <si>
     <t>香藤満月</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>リアラ
-マコトユマ(D引退中)</t>
-    <rPh sb="11" eb="13">
-      <t>インタイ</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>チュウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1454,11 +1421,6 @@
     <rPh sb="5" eb="9">
       <t>インタイヨテイ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ホルスタイン・エンジュ
-ラブリカ・ヒナーノ</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1535,6 +1497,51 @@
     <rPh sb="23" eb="25">
       <t>セカイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ハミングバード
+メガトン
+後藤智香
+天麗皇希
+山田奈保(休)</t>
+    <rPh sb="13" eb="17">
+      <t>ゴトウチカ</t>
+    </rPh>
+    <rPh sb="18" eb="22">
+      <t>アマレイコウキ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>キュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ホルスタイン・エンジュ
+ラブリカ・ヒナーノ
+枢夜 佐季</t>
+    <rPh sb="22" eb="23">
+      <t>クルル</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>サキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>梨央
+(弥福かな)
+(ゴんべ)</t>
+    <rPh sb="0" eb="2">
+      <t>リオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>リアラ</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2427,10 +2434,10 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="T24" sqref="T24"/>
+      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.77734375" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
@@ -2466,7 +2473,7 @@
     <row r="2" spans="1:21" x14ac:dyDescent="0.8">
       <c r="B2" s="1">
         <f>SUM(C2:RU2)</f>
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C2" s="1" cm="1">
         <f t="array" ref="C2">SUMPRODUCT(
@@ -2482,7 +2489,7 @@
      LEN(D5:D999) - LEN(SUBSTITUTE(D5:D999, CHAR(10), "")) + 1
   )
 )</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" cm="1">
         <f t="array" ref="E2">SUMPRODUCT(
@@ -2522,7 +2529,7 @@
      LEN(I5:I999) - LEN(SUBSTITUTE(I5:I999, CHAR(10), "")) + 1
   )
 )</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1" cm="1">
         <f t="array" ref="J2">SUMPRODUCT(
@@ -2618,7 +2625,7 @@
      LEN(U5:U999) - LEN(SUBSTITUTE(U5:U999, CHAR(10), "")) + 1
   )
 )</f>
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="16.7" x14ac:dyDescent="0.8">
@@ -3155,7 +3162,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -3163,7 +3170,7 @@
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="U23" s="3" t="s">
         <v>85</v>
@@ -3454,7 +3461,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -3512,13 +3519,13 @@
         <v>2008</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -3605,7 +3612,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>143</v>
@@ -3645,7 +3652,7 @@
         <v>54</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -3699,10 +3706,10 @@
         <v>137</v>
       </c>
       <c r="T41" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="U41" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="2:21" ht="16.7" x14ac:dyDescent="0.8">
@@ -3766,7 +3773,7 @@
       </c>
       <c r="T43" s="3"/>
       <c r="U43" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="2:21" ht="33.35" x14ac:dyDescent="0.8">
@@ -3790,7 +3797,7 @@
         <v>36</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
@@ -3800,7 +3807,7 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="2:21" ht="33.35" x14ac:dyDescent="0.8">
@@ -3824,7 +3831,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3" t="s">
@@ -3840,7 +3847,7 @@
         <v>75</v>
       </c>
       <c r="U45" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="2:21" ht="100" x14ac:dyDescent="0.8">
@@ -3854,7 +3861,7 @@
         <v>48</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>17</v>
@@ -3894,7 +3901,7 @@
         <v>2019</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
@@ -3916,7 +3923,7 @@
         <v>31</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3" t="s">
@@ -3932,7 +3939,7 @@
         <v>76</v>
       </c>
       <c r="U47" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="2:21" ht="50" x14ac:dyDescent="0.8">
@@ -3952,7 +3959,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3" t="s">
@@ -3969,10 +3976,10 @@
       </c>
       <c r="S48" s="3"/>
       <c r="T48" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="2:21" ht="50" x14ac:dyDescent="0.8">
@@ -4015,7 +4022,7 @@
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
       <c r="T49" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="U49" s="3"/>
     </row>
@@ -4033,10 +4040,10 @@
         <v>52</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>159</v>
+        <v>191</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>103</v>
@@ -4053,7 +4060,7 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
@@ -4091,7 +4098,7 @@
         <v>64</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
@@ -4105,14 +4112,14 @@
         <v>27</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
       <c r="U51" s="3" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="2:21" ht="100" x14ac:dyDescent="0.8">
@@ -4144,10 +4151,10 @@
         <v>32</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
@@ -4155,7 +4162,7 @@
         <v>28</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Q52" s="3" t="s">
         <v>82</v>
@@ -4173,7 +4180,7 @@
         <v>98</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>155</v>
@@ -4186,24 +4193,24 @@
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="U53" s="3"/>
     </row>

</xml_diff>

<commit_message>
Update converter to dynamically read Excel headers and fix column order
- Add extract_promotion_headers() method to read promotion names from Excel
- Add update_html_headers() method to dynamically update HTML table headers
- Fix JTO and チョコプロ column order to match Excel file structure
- HisokA now correctly appears under JTO column as per Excel data
- HTML headers now automatically reflect Excel column order changes

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/woman-excel.xlsx
+++ b/woman-excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wankuma-my.sharepoint.com/personal/naka_wankuma_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\docker-claudecode\2女子プロレスラーの一覧\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="6_{B69F568A-D26F-4418-9710-6ADC08CBB386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D98426-F947-41E5-899B-BFDA0F4288FA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1222C8-5646-4518-A6EF-E84A541CE855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25533" yWindow="-67" windowWidth="25734" windowHeight="13814" xr2:uid="{006E6351-9C88-4E01-B808-191D08DA05AD}"/>
+    <workbookView xWindow="12913" yWindow="1247" windowWidth="12000" windowHeight="9980" xr2:uid="{006E6351-9C88-4E01-B808-191D08DA05AD}"/>
   </bookViews>
   <sheets>
     <sheet name="現役選手デビュー年団体別一覧" sheetId="1" r:id="rId1"/>
@@ -1621,6 +1621,26 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Noto Serif JP SemiBold"/>
+        <family val="1"/>
+        <charset val="128"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1703,26 +1723,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Noto Serif JP SemiBold"/>
-        <family val="1"/>
-        <charset val="128"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2081,10 +2081,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4A34D807-EC26-4518-9852-7FFB26CEC57B}" name="テーブル1" displayName="テーブル1" ref="B4:U53" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="B4:U53" xr:uid="{4A34D807-EC26-4518-9852-7FFB26CEC57B}"/>
@@ -2095,20 +2091,20 @@
     <tableColumn id="22" xr3:uid="{8EA6491D-1F78-431F-AD9B-C8AB4F6616E9}" name="TJPW" dataDxfId="16"/>
     <tableColumn id="3" xr3:uid="{CA5FBB65-FE37-40A8-B1DD-0182D7DD64C3}" name="マリゴ" dataDxfId="15"/>
     <tableColumn id="27" xr3:uid="{50745B86-8D07-4F72-B93E-5C2E105BB03C}" name="IR/ホットシュシュ" dataDxfId="14"/>
+    <tableColumn id="30" xr3:uid="{BB23C0DC-5AEB-431A-A828-4D1BDF4F315F}" name="JTO" dataDxfId="0"/>
     <tableColumn id="29" xr3:uid="{ADFF1D58-E918-4FF6-B352-AA98020CFD16}" name="チョコプロ" dataDxfId="13"/>
-    <tableColumn id="30" xr3:uid="{BB23C0DC-5AEB-431A-A828-4D1BDF4F315F}" name="JTO" dataDxfId="12"/>
-    <tableColumn id="17" xr3:uid="{C0123278-DCF4-45DB-8696-FC0805957C5C}" name="Diana" dataDxfId="11"/>
-    <tableColumn id="32" xr3:uid="{67EA2433-E1D1-4094-BFB4-0EDB7438926B}" name="Pure-J" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{ACF43FBE-31D7-4ED6-A997-E4AF4BF0B9D4}" name="マーベラス" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{9647ED0D-42FB-42C1-BFB2-8B8D56D414C4}" name="SENDAI" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{73103D07-0C18-49E4-833A-41ADC2D3DE61}" name="Wave" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{86389032-6123-44BF-98AB-D3CA13F2577A}" name="LLPW-X" dataDxfId="6"/>
-    <tableColumn id="34" xr3:uid="{C9FDFCD5-EB7A-4498-855C-DD4AF6E60734}" name="2.5" dataDxfId="5"/>
-    <tableColumn id="28" xr3:uid="{8FEFA60F-BAF5-466B-B569-8C96F8534AF7}" name="シード" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{11B98A53-6EA8-44AD-B33B-82B313F30661}" name="ガンプロ" dataDxfId="3"/>
-    <tableColumn id="33" xr3:uid="{56EE63D7-2296-4070-86B8-49B5D171AF20}" name="海外" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{50B4283E-4FFA-4BD0-B17F-8B3414F0E4D2}" name="その他" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{CE5E3F3B-FB92-45D8-AA5E-A154DC9761D3}" name="フリー" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{C0123278-DCF4-45DB-8696-FC0805957C5C}" name="Diana" dataDxfId="12"/>
+    <tableColumn id="32" xr3:uid="{67EA2433-E1D1-4094-BFB4-0EDB7438926B}" name="Pure-J" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{ACF43FBE-31D7-4ED6-A997-E4AF4BF0B9D4}" name="マーベラス" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{9647ED0D-42FB-42C1-BFB2-8B8D56D414C4}" name="SENDAI" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{73103D07-0C18-49E4-833A-41ADC2D3DE61}" name="Wave" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{86389032-6123-44BF-98AB-D3CA13F2577A}" name="LLPW-X" dataDxfId="7"/>
+    <tableColumn id="34" xr3:uid="{C9FDFCD5-EB7A-4498-855C-DD4AF6E60734}" name="2.5" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{8FEFA60F-BAF5-466B-B569-8C96F8534AF7}" name="シード" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{11B98A53-6EA8-44AD-B33B-82B313F30661}" name="ガンプロ" dataDxfId="4"/>
+    <tableColumn id="33" xr3:uid="{56EE63D7-2296-4070-86B8-49B5D171AF20}" name="海外" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{50B4283E-4FFA-4BD0-B17F-8B3414F0E4D2}" name="その他" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{CE5E3F3B-FB92-45D8-AA5E-A154DC9761D3}" name="フリー" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2437,10 +2433,10 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="47.77734375" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="47.77734375" defaultRowHeight="18" x14ac:dyDescent="0.8"/>
   <cols>
     <col min="1" max="1" width="1.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2448,32 +2444,33 @@
     <col min="4" max="4" width="9.71875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.27734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.71875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="47.77734375" style="1"/>
+    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.27734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.71875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="47.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.8">
       <c r="A1" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.8">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" ht="16" x14ac:dyDescent="0.8">
       <c r="B2" s="1">
         <f>SUM(C2:RU2)</f>
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C2" s="1" cm="1">
         <f t="array" ref="C2">SUMPRODUCT(
@@ -2521,7 +2518,7 @@
      LEN(H5:H999) - LEN(SUBSTITUTE(H5:H999, CHAR(10), "")) + 1
   )
 )</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" cm="1">
         <f t="array" ref="I2">SUMPRODUCT(
@@ -2529,104 +2526,107 @@
      LEN(I5:I999) - LEN(SUBSTITUTE(I5:I999, CHAR(10), "")) + 1
   )
 )</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J2" s="1" cm="1">
         <f t="array" ref="J2">SUMPRODUCT(
-  IF(LEN(J5:J999)=0, 0,
-     LEN(J5:J999) - LEN(SUBSTITUTE(J5:J999, CHAR(10), "")) + 1
-  )
-)</f>
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" cm="1">
-        <f t="array" ref="K2">SUMPRODUCT(
   IF(LEN(K5:K999)=0, 0,
      LEN(K5:K999) - LEN(SUBSTITUTE(K5:K999, CHAR(10), "")) + 1
   )
 )</f>
         <v>9</v>
       </c>
-      <c r="L2" s="1" cm="1">
-        <f t="array" ref="L2">SUMPRODUCT(
+      <c r="K2" s="1" cm="1">
+        <f t="array" ref="K2">SUMPRODUCT(
   IF(LEN(L5:L999)=0, 0,
      LEN(L5:L999) - LEN(SUBSTITUTE(L5:L999, CHAR(10), "")) + 1
   )
 )</f>
         <v>9</v>
       </c>
-      <c r="M2" s="1" cm="1">
-        <f t="array" ref="M2">SUMPRODUCT(
+      <c r="L2" s="1" cm="1">
+        <f t="array" ref="L2">SUMPRODUCT(
   IF(LEN(M5:M999)=0, 0,
      LEN(M5:M999) - LEN(SUBSTITUTE(M5:M999, CHAR(10), "")) + 1
   )
 )</f>
         <v>9</v>
       </c>
-      <c r="N2" s="1" cm="1">
-        <f t="array" ref="N2">SUMPRODUCT(
+      <c r="M2" s="1" cm="1">
+        <f t="array" ref="M2">SUMPRODUCT(
   IF(LEN(N5:N999)=0, 0,
      LEN(N5:N999) - LEN(SUBSTITUTE(N5:N999, CHAR(10), "")) + 1
   )
 )</f>
         <v>6</v>
       </c>
-      <c r="O2" s="1" cm="1">
-        <f t="array" ref="O2">SUMPRODUCT(
+      <c r="N2" s="1" cm="1">
+        <f t="array" ref="N2">SUMPRODUCT(
   IF(LEN(O5:O999)=0, 0,
      LEN(O5:O999) - LEN(SUBSTITUTE(O5:O999, CHAR(10), "")) + 1
   )
 )</f>
         <v>5</v>
       </c>
-      <c r="P2" s="1" cm="1">
-        <f t="array" ref="P2">SUMPRODUCT(
+      <c r="O2" s="1" cm="1">
+        <f t="array" ref="O2">SUMPRODUCT(
   IF(LEN(P5:P999)=0, 0,
      LEN(P5:P999) - LEN(SUBSTITUTE(P5:P999, CHAR(10), "")) + 1
   )
 )</f>
         <v>5</v>
       </c>
-      <c r="Q2" s="1" cm="1">
-        <f t="array" ref="Q2">SUMPRODUCT(
+      <c r="P2" s="1" cm="1">
+        <f t="array" ref="P2">SUMPRODUCT(
   IF(LEN(Q5:Q999)=0, 0,
      LEN(Q5:Q999) - LEN(SUBSTITUTE(Q5:Q999, CHAR(10), "")) + 1
   )
 )</f>
         <v>5</v>
       </c>
-      <c r="R2" s="1" cm="1">
-        <f t="array" ref="R2">SUMPRODUCT(
+      <c r="Q2" s="1" cm="1">
+        <f t="array" ref="Q2">SUMPRODUCT(
   IF(LEN(R5:R999)=0, 0,
      LEN(R5:R999) - LEN(SUBSTITUTE(R5:R999, CHAR(10), "")) + 1
   )
 )</f>
         <v>4</v>
       </c>
-      <c r="S2" s="1" cm="1">
-        <f t="array" ref="S2">SUMPRODUCT(
+      <c r="R2" s="1" cm="1">
+        <f t="array" ref="R2">SUMPRODUCT(
   IF(LEN(S5:S999)=0, 0,
      LEN(S5:S999) - LEN(SUBSTITUTE(S5:S999, CHAR(10), "")) + 1
   )
 )</f>
         <v>8</v>
       </c>
-      <c r="T2" s="1" cm="1">
-        <f t="array" ref="T2">SUMPRODUCT(
+      <c r="S2" s="1" cm="1">
+        <f t="array" ref="S2">SUMPRODUCT(
   IF(LEN(T5:T999)=0, 0,
      LEN(T5:T999) - LEN(SUBSTITUTE(T5:T999, CHAR(10), "")) + 1
   )
 )</f>
         <v>29</v>
       </c>
-      <c r="U2" s="1" cm="1">
-        <f t="array" ref="U2">SUMPRODUCT(
+      <c r="T2" s="1" cm="1">
+        <f t="array" ref="T2">SUMPRODUCT(
   IF(LEN(U5:U999)=0, 0,
      LEN(U5:U999) - LEN(SUBSTITUTE(U5:U999, CHAR(10), "")) + 1
   )
 )</f>
         <v>45</v>
       </c>
+      <c r="U2" s="1" cm="1">
+        <f t="array" ref="U2">SUMPRODUCT(
+  IF(LEN(V5:V999)=0, 0,
+     LEN(V5:V999) - LEN(SUBSTITUTE(V5:V999, CHAR(10), "")) + 1
+  )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.8">
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:21" ht="16.7" x14ac:dyDescent="0.8">
       <c r="B4" s="2" t="s">
@@ -2648,10 +2648,10 @@
         <v>110</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>22</v>
@@ -2888,7 +2888,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="16.7" x14ac:dyDescent="0.8">
+    <row r="13" spans="1:21" ht="33.35" x14ac:dyDescent="0.8">
       <c r="B13" s="3">
         <v>1985</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
     </row>
-    <row r="23" spans="2:21" ht="33.35" x14ac:dyDescent="0.8">
+    <row r="23" spans="2:21" ht="66.7" x14ac:dyDescent="0.8">
       <c r="B23" s="3">
         <v>1995</v>
       </c>
@@ -3153,10 +3153,10 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -3258,7 +3258,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="2:21" ht="16.7" x14ac:dyDescent="0.8">
+    <row r="27" spans="2:21" ht="33.35" x14ac:dyDescent="0.8">
       <c r="B27" s="3">
         <v>1999</v>
       </c>
@@ -3344,7 +3344,7 @@
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
     </row>
-    <row r="30" spans="2:21" ht="16.7" x14ac:dyDescent="0.8">
+    <row r="30" spans="2:21" ht="33.35" x14ac:dyDescent="0.8">
       <c r="B30" s="3">
         <v>2002</v>
       </c>
@@ -3581,10 +3581,10 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="3"/>
+      <c r="I38" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -3640,7 +3640,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="2:21" ht="33.35" x14ac:dyDescent="0.8">
+    <row r="40" spans="2:21" ht="50" x14ac:dyDescent="0.8">
       <c r="B40" s="3">
         <v>2012</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="2:21" ht="100" x14ac:dyDescent="0.8">
+    <row r="46" spans="2:21" ht="150" x14ac:dyDescent="0.8">
       <c r="B46" s="3">
         <v>2018</v>
       </c>
@@ -3867,10 +3867,10 @@
         <v>17</v>
       </c>
       <c r="G46" s="3"/>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="3"/>
+      <c r="I46" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
         <v>128</v>
@@ -3914,10 +3914,10 @@
         <v>141</v>
       </c>
       <c r="H47" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>31</v>
@@ -3957,10 +3957,10 @@
         <v>16</v>
       </c>
       <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3" t="s">
+      <c r="H48" s="3" t="s">
         <v>167</v>
       </c>
+      <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3" t="s">
         <v>129</v>
@@ -4001,10 +4001,10 @@
       <c r="G49" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3" t="s">
@@ -4046,10 +4046,10 @@
         <v>177</v>
       </c>
       <c r="H50" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I50" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>30</v>
@@ -4092,10 +4092,10 @@
         <v>154</v>
       </c>
       <c r="H51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>169</v>
@@ -4142,10 +4142,10 @@
         <v>139</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I52" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>32</v>
@@ -4191,10 +4191,10 @@
       <c r="G53" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>192</v>
       </c>
+      <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3" t="s">

</xml_diff>